<commit_message>
0.1.031 : New username generator, updates to monitor
</commit_message>
<xml_diff>
--- a/monitor/userwords.xlsx
+++ b/monitor/userwords.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Everything\Programming\nodejs\Projects\bubbl\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Everything\Programming\nodejs\Projects\bubbl\monitor\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="450" windowWidth="26670" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="900" windowWidth="26670" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33298,8 +33298,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A11011"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A10944" workbookViewId="0">
+      <selection activeCell="Q10960" sqref="Q10960"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>